<commit_message>
Correções do template da planilha. - Correção da formatação da data de validade na planilha resultante de uma requisição
</commit_message>
<xml_diff>
--- a/Files/template.xlsx
+++ b/Files/template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\205072\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anderson\Documents\NetBeansProjects\tcc\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,15 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>NATUREZA DE DESPESA</t>
   </si>
@@ -79,6 +82,15 @@
   </si>
   <si>
     <t>CPV</t>
+  </si>
+  <si>
+    <t>INFORMAÇÕES DO PROCESSO E NATUREZA DE DESPESA</t>
+  </si>
+  <si>
+    <t>INFORMAÇÕES DO ITEM</t>
+  </si>
+  <si>
+    <t>INFORMAÇÕES PÓS-LICITAÇÃO</t>
   </si>
 </sst>
 </file>
@@ -126,7 +138,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -208,12 +220,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -258,6 +279,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -265,8 +295,36 @@
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -541,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:T12"/>
+  <dimension ref="A1:T12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,6 +628,34 @@
     <col min="20" max="20" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+    </row>
     <row r="2" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
@@ -663,6 +749,11 @@
       <c r="I12" s="10"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="J1:N1"/>
+    <mergeCell ref="O1:T1"/>
+  </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>